<commit_message>
feat: resolve requisito 1
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -1228,7 +1228,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>7</v>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4">
         <v>8</v>
       </c>
@@ -1276,7 +1276,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4"/>
       <c r="B22" s="8"/>
       <c r="C22" s="4"/>
@@ -1288,7 +1288,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4"/>
       <c r="B23" s="8"/>
       <c r="C23" s="4"/>
@@ -1300,7 +1300,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4"/>
       <c r="B24" s="8"/>
       <c r="C24" s="4"/>
@@ -1312,7 +1312,7 @@
       <c r="I24" s="4"/>
       <c r="J24" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4"/>
       <c r="B25" s="8"/>
       <c r="C25" s="4"/>
@@ -1324,7 +1324,7 @@
       <c r="I25" s="4"/>
       <c r="J25" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4"/>
       <c r="B26" s="8"/>
       <c r="C26" s="4"/>
@@ -1336,7 +1336,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4"/>
       <c r="B27" s="8"/>
       <c r="C27" s="4"/>

</xml_diff>